<commit_message>
Update multiple students template form
</commit_message>
<xml_diff>
--- a/live/Add_Multiple_Students_Template.xlsx
+++ b/live/Add_Multiple_Students_Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16CB5067-AF77-4D5F-8C69-4ACDEF72FF24}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8DAD138-A4B4-4D17-838C-DADFA41FEDDB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>No</t>
   </si>
@@ -48,6 +48,96 @@
   </si>
   <si>
     <t>site11</t>
+  </si>
+  <si>
+    <t>Server List</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t>am1</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>us1</t>
+  </si>
+  <si>
+    <t>China-1</t>
+  </si>
+  <si>
+    <t>cn1</t>
+  </si>
+  <si>
+    <t>China-2</t>
+  </si>
+  <si>
+    <t>cn2</t>
+  </si>
+  <si>
+    <t>China-3</t>
+  </si>
+  <si>
+    <t>cn3</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>eu1</t>
+  </si>
+  <si>
+    <t>Indonesia-1</t>
+  </si>
+  <si>
+    <t>id1</t>
+  </si>
+  <si>
+    <t>Indonesia-2</t>
+  </si>
+  <si>
+    <t>id2</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>kr1</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>my1</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>mx1</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>mn1</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>mone</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>vn1</t>
   </si>
 </sst>
 </file>
@@ -82,15 +172,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,12 +203,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -124,6 +231,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J4" sqref="J4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,9 +578,11 @@
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1">
+    <row r="1" spans="1:11" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -479,8 +607,9 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -505,16 +634,145 @@
       <c r="H2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="J4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="J5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="J6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="J7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="J8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="J9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="J10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="J11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="J12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="J13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="J14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="J15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="J16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11">
+      <c r="J17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11">
+      <c r="J18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J2:K3"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="nputri@dyned.com" xr:uid="{0699096A-19E8-466B-805B-9D181A17A51F}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{BCCC5E76-6F34-4FD2-81FD-A39E558EB7F0}"/>

</xml_diff>